<commit_message>
Atualizar fontes de dados
</commit_message>
<xml_diff>
--- a/public/data/downside_risk_-_year.xlsx
+++ b/public/data/downside_risk_-_year.xlsx
@@ -595,94 +595,94 @@
         <v>2025</v>
       </c>
       <c r="B2" t="n">
-        <v>3672</v>
+        <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>-6.364814259472764</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>3.825359215686274</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>-10.19017347515904</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>-17.19934640522876</v>
+        <v>0</v>
       </c>
       <c r="G2" t="n">
         <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>-30.99082706993028</v>
+        <v>0</v>
       </c>
       <c r="I2" t="n">
-        <v>41.82535921568628</v>
+        <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>-35779733.78194224</v>
+        <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>-9851708.402352255</v>
+        <v>0</v>
       </c>
       <c r="L2" t="n">
-        <v>-7103128.559472259</v>
+        <v>0</v>
       </c>
       <c r="M2" t="n">
-        <v>323074.53792</v>
+        <v>0</v>
       </c>
       <c r="N2" t="n">
-        <v>-3071654.3808</v>
+        <v>0</v>
       </c>
       <c r="O2" t="n">
-        <v>-45631442.18429451</v>
+        <v>0</v>
       </c>
       <c r="P2" t="n">
-        <v>-3151582.996067189</v>
+        <v>0</v>
       </c>
       <c r="Q2" t="n">
-        <v>-4195440.103160923</v>
+        <v>0</v>
       </c>
       <c r="R2" t="n">
-        <v>-2800860.809589479</v>
+        <v>0</v>
       </c>
       <c r="S2" t="n">
-        <v>-3802983.350393677</v>
+        <v>0</v>
       </c>
       <c r="T2" t="n">
-        <v>-155524.8518937884</v>
+        <v>0</v>
       </c>
       <c r="U2" t="n">
-        <v>-218072.4289129355</v>
+        <v>0</v>
       </c>
       <c r="V2" t="n">
-        <v>-1467171.035105374</v>
+        <v>0</v>
       </c>
       <c r="W2" t="n">
-        <v>-1985514.970305197</v>
+        <v>0</v>
       </c>
       <c r="X2" t="n">
-        <v>-48783025.1803617</v>
+        <v>0</v>
       </c>
       <c r="Y2" t="n">
-        <v>-49826882.28745543</v>
+        <v>0</v>
       </c>
       <c r="Z2" t="n">
-        <v>0.6331694158570289</v>
+        <v>0</v>
       </c>
       <c r="AA2" t="n">
-        <v>0.331672257357259</v>
+        <v>0</v>
       </c>
       <c r="AB2" t="n">
-        <v>0.03515832678571205</v>
+        <v>0</v>
       </c>
       <c r="AC2" t="n">
-        <v>0.6331371940702528</v>
+        <v>0</v>
       </c>
       <c r="AD2" t="n">
-        <v>0.3305571603287144</v>
+        <v>0</v>
       </c>
       <c r="AE2" t="n">
-        <v>0.03630564560103267</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -690,94 +690,94 @@
         <v>2026</v>
       </c>
       <c r="B3" t="n">
-        <v>8760</v>
+        <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>-31.39887671232876</v>
+        <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>-33.39887671232876</v>
+        <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>-62.29967123287671</v>
+        <v>0</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>
       </c>
       <c r="H3" t="n">
-        <v>-0.09939726027397371</v>
+        <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>31.00019178082192</v>
+        <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>32448319.75584922</v>
+        <v>0</v>
       </c>
       <c r="K3" t="n">
-        <v>-80755354.56</v>
+        <v>0</v>
       </c>
       <c r="L3" t="n">
-        <v>-69038594.16</v>
+        <v>0</v>
       </c>
       <c r="M3" t="n">
-        <v>473040</v>
+        <v>0</v>
       </c>
       <c r="N3" t="n">
-        <v>-12189800.4</v>
+        <v>0</v>
       </c>
       <c r="O3" t="n">
-        <v>-48307034.80415079</v>
+        <v>0</v>
       </c>
       <c r="P3" t="n">
-        <v>-6119609.998599664</v>
+        <v>0</v>
       </c>
       <c r="Q3" t="n">
-        <v>-7984760.118122038</v>
+        <v>0</v>
       </c>
       <c r="R3" t="n">
-        <v>-5835154.080893861</v>
+        <v>0</v>
       </c>
       <c r="S3" t="n">
-        <v>-7796855.27637657</v>
+        <v>0</v>
       </c>
       <c r="T3" t="n">
-        <v>-16757.23056925386</v>
+        <v>0</v>
       </c>
       <c r="U3" t="n">
-        <v>-22519.7486827328</v>
+        <v>0</v>
       </c>
       <c r="V3" t="n">
-        <v>-1752782.702817573</v>
+        <v>0</v>
       </c>
       <c r="W3" t="n">
-        <v>-2273472.434645221</v>
+        <v>0</v>
       </c>
       <c r="X3" t="n">
-        <v>-54426644.80275045</v>
+        <v>0</v>
       </c>
       <c r="Y3" t="n">
-        <v>-56291794.92227283</v>
+        <v>0</v>
       </c>
       <c r="Z3" t="n">
-        <v>0.7673095156670543</v>
+        <v>0</v>
       </c>
       <c r="AA3" t="n">
-        <v>0.2304869465524925</v>
+        <v>0</v>
       </c>
       <c r="AB3" t="n">
-        <v>0.002203537780453207</v>
+        <v>0</v>
       </c>
       <c r="AC3" t="n">
-        <v>0.7725129412195465</v>
+        <v>0</v>
       </c>
       <c r="AD3" t="n">
-        <v>0.2252558005777865</v>
+        <v>0</v>
       </c>
       <c r="AE3" t="n">
-        <v>0.002231258202667029</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -785,94 +785,94 @@
         <v>2027</v>
       </c>
       <c r="B4" t="n">
-        <v>8760</v>
+        <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>41.9</v>
+        <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>34.9</v>
+        <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="G4" t="n">
         <v>0</v>
       </c>
       <c r="H4" t="n">
-        <v>39.9</v>
+        <v>0</v>
       </c>
       <c r="I4" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="J4" t="n">
-        <v>-102393126.2427646</v>
+        <v>0</v>
       </c>
       <c r="K4" t="n">
-        <v>70395360</v>
+        <v>0</v>
       </c>
       <c r="L4" t="n">
-        <v>77079240</v>
+        <v>0</v>
       </c>
       <c r="M4" t="n">
-        <v>1839600</v>
+        <v>0</v>
       </c>
       <c r="N4" t="n">
-        <v>-8523480</v>
+        <v>0</v>
       </c>
       <c r="O4" t="n">
-        <v>-31997766.2427646</v>
+        <v>0</v>
       </c>
       <c r="P4" t="n">
-        <v>-4162865.740890441</v>
+        <v>0</v>
       </c>
       <c r="Q4" t="n">
-        <v>-5454143.487459219</v>
+        <v>0</v>
       </c>
       <c r="R4" t="n">
-        <v>-4071245.542026059</v>
+        <v>0</v>
       </c>
       <c r="S4" t="n">
-        <v>-5376293.838841881</v>
+        <v>0</v>
       </c>
       <c r="T4" t="n">
-        <v>-51873.21997142905</v>
+        <v>0</v>
       </c>
       <c r="U4" t="n">
-        <v>-69219.55541659148</v>
+        <v>0</v>
       </c>
       <c r="V4" t="n">
-        <v>-854707.6265570523</v>
+        <v>0</v>
       </c>
       <c r="W4" t="n">
-        <v>-1131763.190340081</v>
+        <v>0</v>
       </c>
       <c r="X4" t="n">
-        <v>-36160631.98365504</v>
+        <v>0</v>
       </c>
       <c r="Y4" t="n">
-        <v>-37451909.73022381</v>
+        <v>0</v>
       </c>
       <c r="Z4" t="n">
-        <v>0.8178761620507754</v>
+        <v>0</v>
       </c>
       <c r="AA4" t="n">
-        <v>0.171702980345452</v>
+        <v>0</v>
       </c>
       <c r="AB4" t="n">
-        <v>0.01042085760377271</v>
+        <v>0</v>
       </c>
       <c r="AC4" t="n">
-        <v>0.8174042507853614</v>
+        <v>0</v>
       </c>
       <c r="AD4" t="n">
-        <v>0.1720717041138629</v>
+        <v>0</v>
       </c>
       <c r="AE4" t="n">
-        <v>0.01052404510077575</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -880,94 +880,94 @@
         <v>2028</v>
       </c>
       <c r="B5" t="n">
-        <v>8784</v>
+        <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>41.9</v>
+        <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>34.9</v>
+        <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="G5" t="n">
         <v>0</v>
       </c>
       <c r="H5" t="n">
-        <v>39.9</v>
+        <v>0</v>
       </c>
       <c r="I5" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="J5" t="n">
-        <v>-102871554.3084968</v>
+        <v>0</v>
       </c>
       <c r="K5" t="n">
-        <v>65568168</v>
+        <v>0</v>
       </c>
       <c r="L5" t="n">
-        <v>68089176</v>
+        <v>0</v>
       </c>
       <c r="M5" t="n">
-        <v>1906128</v>
+        <v>0</v>
       </c>
       <c r="N5" t="n">
-        <v>-4427136</v>
+        <v>0</v>
       </c>
       <c r="O5" t="n">
-        <v>-37303386.3084968</v>
+        <v>0</v>
       </c>
       <c r="P5" t="n">
-        <v>-1747494.191664356</v>
+        <v>0</v>
       </c>
       <c r="Q5" t="n">
-        <v>-2279698.018527351</v>
+        <v>0</v>
       </c>
       <c r="R5" t="n">
-        <v>-1696366.305596608</v>
+        <v>0</v>
       </c>
       <c r="S5" t="n">
-        <v>-2218596.390782984</v>
+        <v>0</v>
       </c>
       <c r="T5" t="n">
-        <v>-55289.69981280511</v>
+        <v>0</v>
       </c>
       <c r="U5" t="n">
-        <v>-74506.31528722626</v>
+        <v>0</v>
       </c>
       <c r="V5" t="n">
-        <v>-418883.2501498017</v>
+        <v>0</v>
       </c>
       <c r="W5" t="n">
-        <v>-555010.3957826175</v>
+        <v>0</v>
       </c>
       <c r="X5" t="n">
-        <v>-39050880.50016115</v>
+        <v>0</v>
       </c>
       <c r="Y5" t="n">
-        <v>-39583084.32702415</v>
+        <v>0</v>
       </c>
       <c r="Z5" t="n">
-        <v>0.7815414078560668</v>
+        <v>0</v>
       </c>
       <c r="AA5" t="n">
-        <v>0.1929857979195502</v>
+        <v>0</v>
       </c>
       <c r="AB5" t="n">
-        <v>0.02547279422438289</v>
+        <v>0</v>
       </c>
       <c r="AC5" t="n">
-        <v>0.7789706066587333</v>
+        <v>0</v>
       </c>
       <c r="AD5" t="n">
-        <v>0.1948695069102269</v>
+        <v>0</v>
       </c>
       <c r="AE5" t="n">
-        <v>0.02615988643103973</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>